<commit_message>
- Show old HRoCast
</commit_message>
<xml_diff>
--- a/Visualisierung/input/Alt/221201_Glycerin Wasser gemische.xlsx
+++ b/Visualisierung/input/Alt/221201_Glycerin Wasser gemische.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Diss\Software\Hiwi\Visualisierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Diss\Software\Hiwi\Visualisierung\input\Alt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -364,6 +364,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000000000000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -530,10 +533,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1930,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2503,7 +2506,7 @@
       <c r="G21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="14">
         <v>920</v>
       </c>
       <c r="I21" s="11" t="s">
@@ -2515,8 +2518,8 @@
       <c r="G22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="10">
-        <v>1000</v>
+      <c r="H22" s="14">
+        <v>7500</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>29</v>
@@ -2526,9 +2529,9 @@
       <c r="G23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="14">
         <f>H24/H22</f>
-        <v>9.9999999999999986E-10</v>
+        <v>2.6666666666666667E-7</v>
       </c>
       <c r="I23" s="11" t="s">
         <v>30</v>
@@ -2538,21 +2541,21 @@
       <c r="G24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="12">
-        <v>9.9999999999999995E-7</v>
+      <c r="H24" s="14">
+        <v>2E-3</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="14">
+      <c r="H25" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="13" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>